<commit_message>
Added EU Flag to each country
</commit_message>
<xml_diff>
--- a/European Countries.xlsx
+++ b/European Countries.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,433 +436,863 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Country</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>population</t>
+          <t>Subregion</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Poplation</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>European Union Association</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jersey</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>100800</v>
+          <t>Albania</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2837743</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Iceland</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>366425</v>
+          <t>Austria</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Central Europe</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>8917205</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Malta</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>525285</v>
+          <t>Belarus</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Eastern Europe</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>9398861</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Montenegro</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>621718</v>
+          <t>Belgium</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>11555997</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>632275</v>
+          <t>Bosnia and Herzegovina</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3280815</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cyprus</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1207361</v>
+          <t>Bulgaria</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6927288</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Estonia</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1331057</v>
+          <t>Croatia</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>4047200</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kosovo</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1775378</v>
+          <t>Cyprus</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Southern Europe</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1207361</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Latvia</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1901548</v>
+          <t>Czechia</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Central Europe</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>10698896</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>2077132</v>
+          <t>Denmark</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>5831404</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Slovenia</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2100126</v>
+          <t>Estonia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1331057</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Moldova</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2617820</v>
+          <t>Finland</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>5530719</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lithuania</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>2794700</v>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>67391582</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Albania</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>2837743</v>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>83240525</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bosnia and Herzegovina</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>3280815</v>
+          <t>Greece</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Southern Europe</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>10715549</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Croatia</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>4047200</v>
+          <t>Hungary</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Central Europe</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>9749763</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ireland</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>4994724</v>
+          <t>Iceland</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>366425</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>European Free Trade Association (EFTA)</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Norway</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>5379475</v>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>4994724</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Slovakia</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>5458827</v>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Southern Europe</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>59554023</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Finland</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>5530719</v>
+          <t>Jersey</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100800</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Denmark</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>5831404</v>
+          <t>Kosovo</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1775378</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Serbia</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>6908224</v>
+          <t>Latvia</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1901548</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>6927288</v>
+          <t>Lithuania</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2794700</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Switzerland</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>8654622</v>
+          <t>Luxembourg</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>632275</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Austria</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>8917205</v>
+          <t>Malta</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Southern Europe</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>525285</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Belarus</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>9398861</v>
+          <t>Moldova</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Eastern Europe</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2617820</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Hungary</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>9749763</v>
+          <t>Montenegro</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>621718</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Portugal</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>10305564</v>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>16655799</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sweden</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>10353442</v>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>2077132</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Czechia</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>10698896</v>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>5379475</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>European Free Trade Association (EFTA)</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Greece</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>10715549</v>
+          <t>Poland</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Central Europe</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>37950802</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Belgium</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>11555997</v>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Southern Europe</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>10305564</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>16655799</v>
+          <t>Romania</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>19286123</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Romania</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>19286123</v>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Eastern Europe</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>144104080</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Poland</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>37950802</v>
+          <t>Serbia</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Southeast Europe</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>6908224</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ukraine</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>44134693</v>
+          <t>Slovakia</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Central Europe</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>5458827</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>47351567</v>
+          <t>Slovenia</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Central Europe</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>2100126</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>59554023</v>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Southern Europe</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>47351567</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>67215293</v>
+          <t>Sweden</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>10353442</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>67391582</v>
+          <t>Switzerland</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Western Europe</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>8654622</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>European Free Trade Association (EFTA)</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>83240525</v>
+          <t>Ukraine</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Eastern Europe</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>44134693</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>144104080</v>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Northern Europe</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>67215293</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>No Association</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>